<commit_message>
Rapport Milieu de Sprint + MAJ Calendrier
</commit_message>
<xml_diff>
--- a/Artéfacts/Artéfacts Sprint 4/Calendrier Sprint 4.xlsx
+++ b/Artéfacts/Artéfacts Sprint 4/Calendrier Sprint 4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\donoc\Desktop\L3 Informatique\Semestre 2\Projet de développement\Artéfacts\Artéfacts Sprint 4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16E7A1FB-2135-4017-A97E-616D768D861C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0A25121-25A5-4A07-B37D-2CC82212CFE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{9DAF1FEF-636C-495F-A4D9-98A6306D3E56}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="39">
   <si>
     <t>LUNDI</t>
   </si>
@@ -142,6 +142,18 @@
   </si>
   <si>
     <t>Test :</t>
+  </si>
+  <si>
+    <t>Tâche terminé le 27/02/2024</t>
+  </si>
+  <si>
+    <t>Tâches terminé le 04/03/2024</t>
+  </si>
+  <si>
+    <t>Tâches terminé le 05/03/2024</t>
+  </si>
+  <si>
+    <t>Suppression d’articles scientifiques non conforme dans notre Corpus</t>
   </si>
 </sst>
 </file>
@@ -234,7 +246,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -250,8 +262,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -568,8 +578,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A25C790B-9A69-420E-ADEC-218324962F86}">
   <dimension ref="A1:Q22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -600,13 +610,13 @@
       <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="J1" s="13" t="s">
+      <c r="I1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="K1" s="1" t="s">
@@ -621,10 +631,10 @@
       <c r="N1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="O1" s="13" t="s">
+      <c r="O1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="P1" s="13" t="s">
+      <c r="P1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="Q1" s="5" t="s">
@@ -633,67 +643,67 @@
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B2" s="1">
-        <f ca="1">TODAY()</f>
+        <f ca="1">TODAY()-8</f>
         <v>45348</v>
       </c>
       <c r="C2" s="1">
-        <f ca="1">TODAY()+1</f>
+        <f ca="1">B2+1</f>
         <v>45349</v>
       </c>
       <c r="D2" s="1">
-        <f ca="1">TODAY()+2</f>
+        <f t="shared" ref="D2:Q2" ca="1" si="0">C2+1</f>
         <v>45350</v>
       </c>
       <c r="E2" s="1">
-        <f ca="1">TODAY()+3</f>
+        <f t="shared" ca="1" si="0"/>
         <v>45351</v>
       </c>
       <c r="F2" s="1">
-        <f ca="1">TODAY()+4</f>
+        <f t="shared" ca="1" si="0"/>
         <v>45352</v>
       </c>
       <c r="G2" s="1">
-        <f ca="1">TODAY()+5</f>
+        <f t="shared" ca="1" si="0"/>
         <v>45353</v>
       </c>
       <c r="H2" s="1">
-        <f ca="1">TODAY()+6</f>
+        <f t="shared" ca="1" si="0"/>
         <v>45354</v>
       </c>
       <c r="I2" s="1">
-        <f ca="1">TODAY()+7</f>
+        <f t="shared" ca="1" si="0"/>
         <v>45355</v>
       </c>
       <c r="J2" s="1">
-        <f ca="1">TODAY()+8</f>
+        <f t="shared" ca="1" si="0"/>
         <v>45356</v>
       </c>
       <c r="K2" s="1">
-        <f ca="1">TODAY()+9</f>
+        <f t="shared" ca="1" si="0"/>
         <v>45357</v>
       </c>
       <c r="L2" s="1">
-        <f ca="1">TODAY()+10</f>
+        <f t="shared" ca="1" si="0"/>
         <v>45358</v>
       </c>
       <c r="M2" s="1">
-        <f ca="1">TODAY()+11</f>
+        <f t="shared" ca="1" si="0"/>
         <v>45359</v>
       </c>
       <c r="N2" s="1">
-        <f ca="1">TODAY()+12</f>
+        <f t="shared" ca="1" si="0"/>
         <v>45360</v>
       </c>
       <c r="O2" s="1">
-        <f ca="1">TODAY()+13</f>
+        <f t="shared" ca="1" si="0"/>
         <v>45361</v>
       </c>
       <c r="P2" s="1">
-        <f ca="1">TODAY()+14</f>
+        <f t="shared" ca="1" si="0"/>
         <v>45362</v>
       </c>
       <c r="Q2" s="1">
-        <f ca="1">TODAY()+15</f>
+        <f t="shared" ca="1" si="0"/>
         <v>45363</v>
       </c>
     </row>
@@ -705,7 +715,7 @@
         <v>13</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -757,8 +767,8 @@
       <c r="B5">
         <v>0</v>
       </c>
-      <c r="C5">
-        <v>0</v>
+      <c r="C5" s="12">
+        <v>1</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -775,11 +785,11 @@
       <c r="H5">
         <v>0</v>
       </c>
-      <c r="I5">
-        <v>0</v>
-      </c>
-      <c r="J5">
-        <v>0</v>
+      <c r="I5" s="8">
+        <v>2</v>
+      </c>
+      <c r="J5" s="9">
+        <v>2</v>
       </c>
       <c r="K5">
         <v>0</v>
@@ -812,23 +822,23 @@
         <v>13</v>
       </c>
       <c r="C7">
-        <f t="shared" ref="C7:H7" si="0">B7+C4-C5</f>
+        <f t="shared" ref="C7:G7" si="1">B7+C4-C5</f>
         <v>13</v>
       </c>
       <c r="D7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>13</v>
       </c>
       <c r="E7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>13</v>
       </c>
       <c r="F7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>13</v>
       </c>
       <c r="G7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>13</v>
       </c>
       <c r="H7">
@@ -837,39 +847,39 @@
       </c>
       <c r="I7">
         <f>H7+I4-I5</f>
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="J7">
         <f>I7+J4-J5</f>
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="K7">
         <f>J7+K4-K5</f>
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="L7">
-        <f t="shared" ref="J7:Q7" si="1">K7+L4-L5</f>
-        <v>13</v>
+        <f t="shared" ref="L7:Q7" si="2">K7+L4-L5</f>
+        <v>9</v>
       </c>
       <c r="M7">
-        <f t="shared" si="1"/>
-        <v>13</v>
+        <f t="shared" si="2"/>
+        <v>9</v>
       </c>
       <c r="N7">
-        <f t="shared" si="1"/>
-        <v>13</v>
+        <f t="shared" si="2"/>
+        <v>9</v>
       </c>
       <c r="O7">
-        <f t="shared" si="1"/>
-        <v>13</v>
+        <f t="shared" si="2"/>
+        <v>9</v>
       </c>
       <c r="P7">
-        <f t="shared" si="1"/>
-        <v>13</v>
+        <f t="shared" si="2"/>
+        <v>9</v>
       </c>
       <c r="Q7">
-        <f t="shared" si="1"/>
-        <v>13</v>
+        <f t="shared" si="2"/>
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.3">
@@ -898,19 +908,19 @@
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="12"/>
       <c r="B19" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="8"/>
       <c r="B20" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="9"/>
       <c r="B21" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
@@ -928,10 +938,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA30D50F-0BD7-4D6D-98EF-6C8A8DFFE157}">
-  <dimension ref="A1:B24"/>
+  <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -954,7 +964,7 @@
       <c r="A4" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="14">
+      <c r="B4">
         <v>1</v>
       </c>
     </row>
@@ -962,7 +972,7 @@
       <c r="A5" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="14">
+      <c r="B5" s="8">
         <v>1</v>
       </c>
     </row>
@@ -970,7 +980,7 @@
       <c r="A6" t="s">
         <v>25</v>
       </c>
-      <c r="B6" s="14">
+      <c r="B6">
         <v>1</v>
       </c>
     </row>
@@ -978,7 +988,7 @@
       <c r="A7" t="s">
         <v>26</v>
       </c>
-      <c r="B7" s="14">
+      <c r="B7">
         <v>1</v>
       </c>
     </row>
@@ -986,7 +996,7 @@
       <c r="A8" t="s">
         <v>27</v>
       </c>
-      <c r="B8" s="14">
+      <c r="B8">
         <v>1</v>
       </c>
     </row>
@@ -994,7 +1004,7 @@
       <c r="A9" t="s">
         <v>28</v>
       </c>
-      <c r="B9" s="14">
+      <c r="B9" s="9">
         <v>1</v>
       </c>
     </row>
@@ -1002,92 +1012,88 @@
       <c r="A10" t="s">
         <v>29</v>
       </c>
-      <c r="B10" s="14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B11" s="14"/>
+      <c r="B10">
+        <v>1</v>
+      </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>34</v>
       </c>
-      <c r="B12" s="14"/>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B14" s="14"/>
+      <c r="B13">
+        <v>1</v>
+      </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="14"/>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>31</v>
       </c>
-      <c r="B16" s="14">
+      <c r="B16" s="8">
         <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B17" s="14"/>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>21</v>
-      </c>
-      <c r="B18" s="14"/>
+      <c r="A17" t="s">
+        <v>38</v>
+      </c>
+      <c r="B17" s="12">
+        <v>1</v>
+      </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>15</v>
-      </c>
-      <c r="B19" s="14">
-        <v>1</v>
+        <v>21</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>16</v>
-      </c>
-      <c r="B20" s="14">
+        <v>15</v>
+      </c>
+      <c r="B20">
         <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>32</v>
-      </c>
-      <c r="B21" s="14">
+        <v>16</v>
+      </c>
+      <c r="B21">
         <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
+        <v>32</v>
+      </c>
+      <c r="B22" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
         <v>17</v>
       </c>
-      <c r="B22" s="14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A24" s="10" t="s">
+      <c r="B23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="B24">
-        <f>B4+B5+B6+B7+B8+B9+B10+B13+B16+B19+B20+B21+B22</f>
-        <v>13</v>
+      <c r="B25">
+        <f>B4+B5+B6+B7+B8+B9+B10+B13+B16+B17+B20+B21+B22+B23</f>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>